<commit_message>
End of meeting xlsx roles
</commit_message>
<xml_diff>
--- a/Meetings/21 Feb/Roles.xlsx
+++ b/Meetings/21 Feb/Roles.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
-    <sheet name="New" sheetId="3" r:id="rId2"/>
-    <sheet name="Projection" sheetId="2" r:id="rId3"/>
+    <sheet name="Finished" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Alexandre</t>
   </si>
@@ -98,7 +97,7 @@
     <t>Current State</t>
   </si>
   <si>
-    <t>Possible Projection</t>
+    <t>Finished Version</t>
   </si>
 </sst>
 </file>
@@ -241,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -255,7 +254,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -263,11 +261,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -322,42 +316,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau37" displayName="Tableau37" ref="B4:M16" totalsRowShown="0">
-  <autoFilter ref="B4:M16">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="12">
-    <tableColumn id="1" name="Job"/>
-    <tableColumn id="2" name="Vytas"/>
-    <tableColumn id="3" name="Robert"/>
-    <tableColumn id="4" name="Olivia"/>
-    <tableColumn id="5" name="Beenita"/>
-    <tableColumn id="6" name="Jakub"/>
-    <tableColumn id="7" name="Juliano"/>
-    <tableColumn id="8" name="Alexandre"/>
-    <tableColumn id="9" name="Mitchell"/>
-    <tableColumn id="10" name="Anushan"/>
-    <tableColumn id="12" name=" "/>
-    <tableColumn id="11" name="STATUS" dataDxfId="0">
-      <calculatedColumnFormula>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau36" displayName="Tableau36" ref="B4:M16" totalsRowShown="0">
   <autoFilter ref="B4:M16">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -656,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -680,20 +638,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -997,248 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="6">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="11">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="11">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16">
-        <f>IF(SUM(Tableau37[[#This Row],[Vytas]:[Anushan]])=0,5,AVERAGE(Tableau37[[#This Row],[Vytas]:[Anushan]]))</f>
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:M2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C5:L16">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M16">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:K4"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,20 +976,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">

</xml_diff>